<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٠:٥٣ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,9 +454,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٠:٤٤ م</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C3" t="str">
+        <v>2222</v>
+      </c>
+      <c r="D3" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E3" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F3" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G3" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H3" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٠:٥٣ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٢:٥١ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٠:٥٣ م</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C4" t="str">
+        <v>2222</v>
+      </c>
+      <c r="D4" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E4" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F4" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G4" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H4" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٢:٥١ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٦:٠٣ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٢:٥١ م</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C5" t="str">
+        <v>2222</v>
+      </c>
+      <c r="D5" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F5" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G5" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H5" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٦:٠٣ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٧:٥٧ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٦:٠٣ م</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C6" t="str">
+        <v>2222</v>
+      </c>
+      <c r="D6" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F6" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G6" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H6" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٧:٥٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٠:٣٥ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,9 +558,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠١:٥٧:٥٧ م</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve">حسن </v>
+      </c>
+      <c r="C7" t="str">
+        <v>2222</v>
+      </c>
+      <c r="D7" t="str">
+        <v>ايتا</v>
+      </c>
+      <c r="E7" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F7" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G7" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H7" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٠:٣٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٢:١٧ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -584,9 +584,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٠:٣٥ م</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v>حسن</v>
+      </c>
+      <c r="C8" t="str">
+        <v>222</v>
+      </c>
+      <c r="D8" t="str">
+        <v>النصر</v>
+      </c>
+      <c r="E8" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F8" t="str">
+        <v>C5</v>
+      </c>
+      <c r="G8" t="str">
+        <v>WCK</v>
+      </c>
+      <c r="H8" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٢:١٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٩:٣٨ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,9 +610,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٢:١٧ م</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <v>أحمد شريم</v>
+      </c>
+      <c r="C9" t="str">
+        <v>333</v>
+      </c>
+      <c r="D9" t="str">
+        <v>النصر</v>
+      </c>
+      <c r="E9" t="str">
+        <v>الرحلة 3</v>
+      </c>
+      <c r="F9" t="str">
+        <v>C5</v>
+      </c>
+      <c r="G9" t="str">
+        <v>WCK</v>
+      </c>
+      <c r="H9" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٩:٣٨ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠٢:١٠:٣٦ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,9 +636,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٠٩:٣٨ م</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C10" t="str">
+        <v>222</v>
+      </c>
+      <c r="D10" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E10" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F10" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G10" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H10" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:١٠:٣٦ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-02.xlsx at ٠٢‏/٠٥‏/٢٠٢٥ ٠٢:١٣:٤٩ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -662,9 +662,35 @@
         <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:١٠:٣٦ م</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v>يامن</v>
+      </c>
+      <c r="C11" t="str">
+        <v>23</v>
+      </c>
+      <c r="D11" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E11" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F11" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G11" t="str">
+        <v>NRC</v>
+      </c>
+      <c r="H11" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:١٣:٤٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append 1 rows at 2025-05-02T11:40:55.568Z
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-02.xlsx
+++ b/Database/Report-2025-05-02.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -714,9 +714,35 @@
         <v>٢‏/٥‏/٢٠٢٥ ٢:٣٧:٤٣ م</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C13" t="str">
+        <v>222</v>
+      </c>
+      <c r="D13" t="str">
+        <v>الجزائري</v>
+      </c>
+      <c r="E13" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F13" t="str">
+        <v>C3</v>
+      </c>
+      <c r="G13" t="str">
+        <v>WCK</v>
+      </c>
+      <c r="H13" t="str">
+        <v>٠٢‏/٠٥‏/٢٠٢٥ ٠٢:٤٠:٥٥ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>